<commit_message>
HF: Updated with POM
</commit_message>
<xml_diff>
--- a/seleniumTestShopDDT/src/test/resources/data.xlsx
+++ b/seleniumTestShopDDT/src/test/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\Documents\SeleniumTests\seleniumTestShopDDT\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B4203E-EC9E-4877-B1F4-A10BC78EC285}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C9A4C9-6C36-4718-AA7C-C283B5E52DEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="3540" windowWidth="16200" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,16 +69,16 @@
     <t>acfff</t>
   </si>
   <si>
-    <t>fbjj@izzum.com</t>
-  </si>
-  <si>
-    <t>jjfs@gsc.com</t>
-  </si>
-  <si>
-    <t>jdf@sdfgdf.com</t>
-  </si>
-  <si>
-    <t>hh@gsfd.com</t>
+    <t>test1@izzum.com</t>
+  </si>
+  <si>
+    <t>test2@gsc.com</t>
+  </si>
+  <si>
+    <t>test3@sdfgdf.com</t>
+  </si>
+  <si>
+    <t>test4@gsfd.com</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
HF: Adding test results to xlsx
</commit_message>
<xml_diff>
--- a/seleniumTestShopDDT/src/test/resources/data.xlsx
+++ b/seleniumTestShopDDT/src/test/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\Documents\SeleniumTests\seleniumTestShopDDT\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C9A4C9-6C36-4718-AA7C-C283B5E52DEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5555B04D-854E-4923-9FFE-64277B471DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="3540" windowWidth="16200" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,16 +69,16 @@
     <t>acfff</t>
   </si>
   <si>
-    <t>test1@izzum.com</t>
-  </si>
-  <si>
-    <t>test2@gsc.com</t>
-  </si>
-  <si>
-    <t>test3@sdfgdf.com</t>
-  </si>
-  <si>
-    <t>test4@gsfd.com</t>
+    <t>23931@iz64z8um.com</t>
+  </si>
+  <si>
+    <t>438361@g6s48c.com</t>
+  </si>
+  <si>
+    <t>st3761@sd86fg4df.com</t>
+  </si>
+  <si>
+    <t>593813@g8sf46d.com</t>
   </si>
 </sst>
 </file>
@@ -408,21 +408,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="25.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="7" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -447,8 +447,11 @@
       <c r="H1" s="1">
         <v>47384375648</v>
       </c>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -474,7 +477,7 @@
         <v>47384375648</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -500,7 +503,7 @@
         <v>47384375648</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>

</xml_diff>